<commit_message>
redmine #9276 Cal sheets for GI01SUMO, GI02HYPM, GI03FLMA, GI03FLMB deployments 1 & 2 added/changed in repo.
</commit_message>
<xml_diff>
--- a/GI02HYPM/Omaha_Cal_Info_GI02HYPM_00001.xlsx
+++ b/GI02HYPM/Omaha_Cal_Info_GI02HYPM_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="4515" windowWidth="25230" windowHeight="8100" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="680" windowWidth="24480" windowHeight="12640"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,12 +17,17 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Ref Des</t>
   </si>
@@ -144,16 +149,43 @@
     <t>GI02HYPM-MFC04-01-ZPLSGA000 unit not deployed</t>
   </si>
   <si>
-    <t>GI02HYPM-GP001-00-ENG000000</t>
-  </si>
-  <si>
-    <t>GI02HYPM-WFP02-00-ENG000000</t>
-  </si>
-  <si>
     <t>GI02HYPM</t>
   </si>
   <si>
     <t>GI02HYPM-RIM01-02-CTDMOG090</t>
+  </si>
+  <si>
+    <t>13104-01</t>
+  </si>
+  <si>
+    <t>37-12190</t>
+  </si>
+  <si>
+    <t>GI02HYPM-RIM01-00-SIOENG-000</t>
+  </si>
+  <si>
+    <r>
+      <t>GI02HYPM-WFP02-00-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WFPENG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -161,12 +193,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +351,28 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,16 +451,16 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -424,7 +478,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -487,14 +541,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -556,8 +610,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -580,19 +640,19 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -616,10 +676,10 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -632,11 +692,18 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="137">
     <cellStyle name="Comma 2" xfId="62"/>
     <cellStyle name="Comma 2 2" xfId="63"/>
     <cellStyle name="Comma 2 2 2" xfId="64"/>
@@ -647,6 +714,12 @@
     <cellStyle name="Currency 2 3" xfId="69"/>
     <cellStyle name="Excel Built-in Normal" xfId="5"/>
     <cellStyle name="Excel Built-in Normal 2" xfId="70"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="8"/>
     <cellStyle name="Hyperlink 2 2" xfId="71"/>
     <cellStyle name="Hyperlink 2 3" xfId="72"/>
@@ -783,7 +856,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1088,29 +1161,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="28">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1145,9 +1218,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="13" customFormat="1">
       <c r="A2" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>30</v>
@@ -1161,7 +1234,9 @@
       <c r="E2" s="17">
         <v>0.71736111111111101</v>
       </c>
-      <c r="F2" s="21"/>
+      <c r="F2" s="28">
+        <v>42232</v>
+      </c>
       <c r="G2" s="16" t="s">
         <v>36</v>
       </c>
@@ -1184,51 +1259,56 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="13" customFormat="1">
       <c r="D3" s="19"/>
       <c r="E3" s="20"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" customFormat="1"/>
+    <row r="5" spans="1:13" customFormat="1"/>
+    <row r="6" spans="1:13" s="13" customFormat="1">
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="13" customFormat="1">
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="13" customFormat="1">
       <c r="D8" s="19"/>
       <c r="E8" s="20"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="13" customFormat="1">
       <c r="D9" s="19"/>
       <c r="E9" s="20"/>
       <c r="F9" s="19"/>
     </row>
-    <row r="10" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="13" customFormat="1">
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
       <c r="F10" s="19"/>
     </row>
-    <row r="11" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="13" customFormat="1">
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
       <c r="F11" s="19"/>
     </row>
-    <row r="12" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="13" customFormat="1">
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
       <c r="F12" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1236,23 +1316,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="78.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="78.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="10" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1275,8 +1355,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="10" customFormat="1" ht="13.9" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="10" customFormat="1"/>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1299,7 +1379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1319,7 +1399,7 @@
         <v>1.415E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1339,7 +1419,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1359,7 +1439,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1382,7 +1462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1405,7 +1485,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1421,14 +1501,14 @@
       <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="1">
-        <v>1.1299999999999999</v>
+      <c r="F9" s="27">
+        <v>1.0960000000000001</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1451,7 +1531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1474,7 +1554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1494,7 +1574,7 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1514,7 +1594,7 @@
         <v>59.975333333333332</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1534,7 +1614,7 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1554,7 +1634,7 @@
         <v>59.975333333333332</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1574,23 +1654,23 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="G21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="27" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>12190</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>5</v>
@@ -1599,18 +1679,18 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="27" t="s">
         <v>43</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>12190</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>6</v>
@@ -1619,18 +1699,18 @@
         <v>59.975333333333332</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>43</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>12190</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>7</v>
@@ -1639,9 +1719,9 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
-        <v>40</v>
+    <row r="27" spans="1:7">
+      <c r="A27" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>30</v>
@@ -1656,9 +1736,9 @@
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="22" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>30</v>
@@ -1666,40 +1746,45 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="26">
-        <v>1327721</v>
+      <c r="D28" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="G28" s="24"/>
     </row>
-    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33"/>
     </row>
-    <row r="34" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34"/>
     </row>
-    <row r="35" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35"/>
     </row>
-    <row r="36" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36"/>
     </row>
-    <row r="37" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37"/>
     </row>
-    <row r="38" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38"/>
     </row>
-    <row r="39" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39"/>
     </row>
-    <row r="40" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40"/>
     </row>
-    <row r="41" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>